<commit_message>
perbaikan bug create pre/posttest
</commit_message>
<xml_diff>
--- a/kms-fe/public/template.xlsx
+++ b/kms-fe/public/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Manajemen Informatika\Kuliah\Semester 4\KMS\KMS_FE\kms-fe\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A79316-35BC-4A6E-926D-DB705B1A608F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C44775C-244D-477D-8D3C-BBCD4895F18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7BCF6A21-73E3-4667-B9AC-727DCDF25687}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>No</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Soal</t>
   </si>
   <si>
-    <t>Bobot</t>
-  </si>
-  <si>
-    <t>Kunci Jawaban</t>
-  </si>
-  <si>
     <t>Pilihan Jawaban</t>
   </si>
   <si>
@@ -48,40 +42,31 @@
     <t>Manakah dari berikut ini yang TIDAK termasuk jenis algoritma Machine Learning?</t>
   </si>
   <si>
-    <t>Multiple Choise</t>
-  </si>
-  <si>
-    <t>Supervised Learning,Unsupervised Learning,Reinforcement Learning,Deep Learning</t>
-  </si>
-  <si>
-    <t>Deep Learning</t>
-  </si>
-  <si>
     <t>Jelaskan bagaimana algoritma Decision Tree digunakan untuk membuat model Machine Learning.</t>
   </si>
   <si>
     <t>Essay</t>
   </si>
   <si>
-    <t>Sistem deteksi spam email</t>
-  </si>
-  <si>
-    <t>Jelaskan pengertian JVM</t>
-  </si>
-  <si>
-    <t>Java Virtual Machine</t>
-  </si>
-  <si>
-    <t>Apa itu Laravel?</t>
-  </si>
-  <si>
-    <t>Framework dalam PHP</t>
-  </si>
-  <si>
-    <t>Buatlah Recycler View!</t>
+    <t>5,0,0,0</t>
+  </si>
+  <si>
+    <t>Pilgan</t>
   </si>
   <si>
     <t>Praktikum</t>
+  </si>
+  <si>
+    <t>Bobot Pilgan</t>
+  </si>
+  <si>
+    <t>Bobot Essay Praktikum</t>
+  </si>
+  <si>
+    <t>Supervised Learning,Unsupervised Learning,Reinforcement Learning, Deep Learning</t>
+  </si>
+  <si>
+    <t>Buatkan program java dengan tema apotek!</t>
   </si>
 </sst>
 </file>
@@ -465,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB62D5FB-B7E1-41E2-A16F-8EE0975BDB54}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,7 +462,7 @@
     <col min="2" max="2" width="64.44140625" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="131.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
     <col min="6" max="6" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
@@ -510,16 +495,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -527,19 +512,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -547,16 +529,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
         <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -567,41 +546,10 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5">
         <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>